<commit_message>
Update format of tables and logfile with new code
Update the descriptives and regression analysis folder
</commit_message>
<xml_diff>
--- a/01. Descriptives/out/Table 1.xlsx
+++ b/01. Descriptives/out/Table 1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="30">
   <si>
     <t>Female</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>freq_tot</t>
+  </si>
+  <si>
+    <t>share</t>
   </si>
 </sst>
 </file>
@@ -136,282 +148,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D26"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>28280</v>
-      </c>
-      <c r="C1" s="1">
-        <v>216636</v>
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>18445</v>
+        <v>28280</v>
       </c>
       <c r="C2" s="1">
-        <v>232487</v>
+        <v>216636</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.13054154813289642</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>8657</v>
+        <v>18445</v>
       </c>
       <c r="C3" s="1">
-        <v>34390</v>
+        <v>232487</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.079337768256664276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>11572</v>
+        <v>8657</v>
       </c>
       <c r="C4" s="1">
-        <v>100108</v>
+        <v>34390</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.25173014402389526</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>10099</v>
+        <v>11572</v>
       </c>
       <c r="C5" s="1">
-        <v>128761</v>
+        <v>100108</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.11559515446424484</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>10897</v>
+        <v>10099</v>
       </c>
       <c r="C6" s="1">
-        <v>129023</v>
+        <v>128761</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.078432135283946991</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>4523</v>
+        <v>10897</v>
       </c>
       <c r="C7" s="1">
-        <v>46124</v>
+        <v>129023</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.084457807242870331</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>7359</v>
+        <v>4523</v>
       </c>
       <c r="C8" s="1">
-        <v>95303</v>
+        <v>46124</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.098061747848987579</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>5923</v>
+        <v>7359</v>
       </c>
       <c r="C9" s="1">
-        <v>90694</v>
+        <v>95303</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.077216878533363342</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>29400</v>
+        <v>5923</v>
       </c>
       <c r="C10" s="1">
-        <v>131045</v>
+        <v>90694</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.06530752032995224</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>4043</v>
+        <v>29400</v>
       </c>
       <c r="C11" s="1">
-        <v>132081</v>
+        <v>131045</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.22435040771961212</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>2300</v>
+        <v>4043</v>
       </c>
       <c r="C12" s="1">
-        <v>34899</v>
+        <v>132081</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.030610004439949989</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>4963</v>
+        <v>2300</v>
       </c>
       <c r="C13" s="1">
-        <v>36812</v>
+        <v>34899</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.065904468297958374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>6557</v>
+        <v>4963</v>
       </c>
       <c r="C14" s="1">
-        <v>75774</v>
+        <v>36812</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.13482016324996948</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>1164</v>
+        <v>6557</v>
       </c>
       <c r="C15" s="1">
-        <v>26155</v>
+        <v>75774</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.086533635854721069</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>1768</v>
+        <v>1164</v>
       </c>
       <c r="C16" s="1">
-        <v>23462</v>
+        <v>26155</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.044503919780254364</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>750</v>
+        <v>1768</v>
       </c>
       <c r="C17" s="1">
-        <v>13343</v>
+        <v>23462</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.075355894863605499</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>14489</v>
+        <v>750</v>
       </c>
       <c r="C18" s="1">
-        <v>29298</v>
+        <v>13343</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.056209247559309006</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>2946</v>
+        <v>14489</v>
       </c>
       <c r="C19" s="1">
-        <v>37250</v>
+        <v>29298</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.49453887343406677</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>2431</v>
+        <v>2946</v>
       </c>
       <c r="C20" s="1">
-        <v>61852</v>
+        <v>37250</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.079087249934673309</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>875</v>
+        <v>2431</v>
       </c>
       <c r="C21" s="1">
-        <v>16101</v>
+        <v>61852</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.039303500205278397</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>1953</v>
+        <v>875</v>
       </c>
       <c r="C22" s="1">
-        <v>22616</v>
+        <v>16101</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.054344449192285538</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>2074</v>
+        <v>1953</v>
       </c>
       <c r="C23" s="1">
-        <v>42353</v>
+        <v>22616</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.08635479211807251</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>3433</v>
+        <v>2074</v>
       </c>
       <c r="C24" s="1">
-        <v>7917</v>
+        <v>42353</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.04896937683224678</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3433</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7917</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.43362385034561157</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>1022</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>21291</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.048001501709222794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>